<commit_message>
Investor advisor incremental changes (#320)
* Random password for users getting created, Confirmed accounts and default advisor view

* Rubocop fix

---------

Co-authored-by: Abhay Chauhan <abhaychauhan@Abhays-MacBook-Air.local>
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_advisors.xlsx
+++ b/public/sample_uploads/investor_advisors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t xml:space="preserve">Email *</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
   </si>
   <si>
     <t xml:space="preserve">terrie@hansen-inc.com</t>
@@ -193,6 +190,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -201,11 +202,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -465,97 +462,95 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1:H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests to verify InvAdv access
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_advisors.xlsx
+++ b/public/sample_uploads/investor_advisors.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408C8022-BC4A-4757-A727-82D88D4D5DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="23985" windowHeight="14265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,88 +25,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">Email *</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investor *</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advisor Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">terrie@hansen-inc.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investor 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAAS Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jeanice@hansen-inc.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investor 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tameika@hansen-inc.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investor 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">daisey@hansen-inc.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investor 4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+  <si>
+    <t>Email *</t>
+  </si>
+  <si>
+    <t>Investor *</t>
+  </si>
+  <si>
+    <t>Add To</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Advisor Entity</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>terrie@hansen-inc.com</t>
+  </si>
+  <si>
+    <t>Investor 1</t>
+  </si>
+  <si>
+    <t>Fund</t>
+  </si>
+  <si>
+    <t>SAAS Fund</t>
+  </si>
+  <si>
+    <t>jeanice@hansen-inc.com</t>
+  </si>
+  <si>
+    <t>Investor 2</t>
+  </si>
+  <si>
+    <t>tameika@hansen-inc.com</t>
+  </si>
+  <si>
+    <t>Investor 3</t>
+  </si>
+  <si>
+    <t>daisey@hansen-inc.com</t>
+  </si>
+  <si>
+    <t>Investor 4</t>
+  </si>
+  <si>
+    <t>Allowed Roles</t>
+  </si>
+  <si>
+    <t>Investor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -116,7 +109,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -133,7 +126,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -141,85 +134,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="6">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Normal 2" xfId="21"/>
-    <cellStyle name="Normal 3" xfId="22"/>
-    <cellStyle name="Normal 4" xfId="23"/>
-    <cellStyle name="Normal 5" xfId="24"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 5" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -278,60 +216,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -363,7 +317,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -387,7 +341,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -447,122 +401,133 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.14"/>
+    <col min="1" max="1" width="21.265625" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" customWidth="1"/>
+    <col min="4" max="4" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="terrie@hansen-inc.com"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{9540D112-375B-41EE-8C10-BB70DD63B981}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>